<commit_message>
BetaPhase 0.1.1 | Imagens para animação incluídas e prontas para serem animadas
</commit_message>
<xml_diff>
--- a/Calculadora.xlsx
+++ b/Calculadora.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\Portfolio_New\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69C3F275-8994-4EC7-9926-90EC98A6D5A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79F46BB9-58E3-4FEE-BFDF-B7AA3485D553}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{EE0BA97B-31A7-4065-886E-C383CEE81F9D}"/>
   </bookViews>
@@ -294,10 +294,22 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="10" fontId="6" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="6" fillId="7" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="2" fontId="6" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="6" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -322,18 +334,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="6" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="6" fillId="7" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -653,7 +653,7 @@
   <dimension ref="A1:L23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:K6"/>
+      <selection activeCell="A8" sqref="A8:K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -667,14 +667,14 @@
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
-      <c r="E1" s="14" t="s">
+      <c r="E1" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="F1" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14" t="s">
+      <c r="G1" s="18"/>
+      <c r="H1" s="18" t="s">
         <v>4</v>
       </c>
       <c r="I1" s="2"/>
@@ -687,10 +687,10 @@
       <c r="B2" s="3"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
@@ -704,13 +704,13 @@
       <c r="E3" s="4">
         <v>678</v>
       </c>
-      <c r="F3" s="16">
+      <c r="F3" s="20">
         <f>(H3/E3)</f>
-        <v>3.1415929203539825</v>
-      </c>
-      <c r="G3" s="17"/>
+        <v>1.0516224188790559</v>
+      </c>
+      <c r="G3" s="21"/>
       <c r="H3" s="5">
-        <v>2130</v>
+        <v>713</v>
       </c>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
@@ -722,95 +722,95 @@
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
-      <c r="E4" s="11" t="s">
+      <c r="E4" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11" t="s">
+      <c r="F4" s="15"/>
+      <c r="G4" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="H4" s="11"/>
+      <c r="H4" s="15"/>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
     </row>
     <row r="5" spans="1:12" ht="27.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A5" s="20" t="s">
+      <c r="A5" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="20"/>
+      <c r="B5" s="12"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
-      <c r="E5" s="12">
+      <c r="E5" s="16">
         <v>136</v>
       </c>
-      <c r="F5" s="13"/>
-      <c r="G5" s="8">
+      <c r="F5" s="17"/>
+      <c r="G5" s="10">
         <f>(E5*F3)</f>
-        <v>427.25663716814165</v>
-      </c>
-      <c r="H5" s="9"/>
+        <v>143.02064896755161</v>
+      </c>
+      <c r="H5" s="11"/>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
       <c r="L5" s="2"/>
     </row>
     <row r="6" spans="1:12" ht="8.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="10"/>
-      <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="10"/>
-      <c r="J6" s="10"/>
-      <c r="K6" s="10"/>
+      <c r="A6" s="14"/>
+      <c r="B6" s="14"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="14"/>
+      <c r="K6" s="14"/>
       <c r="L6" s="2"/>
     </row>
     <row r="7" spans="1:12" ht="27.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A7" s="20" t="s">
+      <c r="A7" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="21"/>
-      <c r="C7" s="18">
-        <v>0.3</v>
-      </c>
-      <c r="D7" s="19"/>
-      <c r="E7" s="8">
+      <c r="B7" s="13"/>
+      <c r="C7" s="8">
+        <v>0.4</v>
+      </c>
+      <c r="D7" s="9"/>
+      <c r="E7" s="10">
         <f>(E3*C7)</f>
-        <v>203.4</v>
-      </c>
-      <c r="F7" s="9"/>
-      <c r="G7" s="8">
+        <v>271.2</v>
+      </c>
+      <c r="F7" s="11"/>
+      <c r="G7" s="10">
         <f>((E3*C7)*F3)</f>
-        <v>639.00000000000011</v>
-      </c>
-      <c r="H7" s="9"/>
+        <v>285.19999999999993</v>
+      </c>
+      <c r="H7" s="11"/>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
     </row>
     <row r="8" spans="1:12" ht="8.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="10"/>
-      <c r="B8" s="10"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="10"/>
-      <c r="I8" s="10"/>
-      <c r="J8" s="10"/>
-      <c r="K8" s="10"/>
+      <c r="A8" s="14"/>
+      <c r="B8" s="14"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="14"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="14"/>
+      <c r="K8" s="14"/>
       <c r="L8" s="2"/>
     </row>
     <row r="9" spans="1:12" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A9" s="20"/>
-      <c r="B9" s="20"/>
+      <c r="A9" s="12"/>
+      <c r="B9" s="12"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
@@ -1016,12 +1016,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A8:K8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="G7:H7"/>
     <mergeCell ref="G5:H5"/>
     <mergeCell ref="A6:K6"/>
     <mergeCell ref="E4:F4"/>
@@ -1032,6 +1026,12 @@
     <mergeCell ref="F3:G3"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="G4:H4"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:K8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="G7:H7"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
BetaPhase 0.1.1 | Imagens e viewport prontos para animação
</commit_message>
<xml_diff>
--- a/Calculadora.xlsx
+++ b/Calculadora.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\Portfolio_New\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69C3F275-8994-4EC7-9926-90EC98A6D5A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79F46BB9-58E3-4FEE-BFDF-B7AA3485D553}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{EE0BA97B-31A7-4065-886E-C383CEE81F9D}"/>
   </bookViews>
@@ -294,10 +294,22 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="10" fontId="6" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="6" fillId="7" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="2" fontId="6" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="6" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -322,18 +334,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="6" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="6" fillId="7" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -653,7 +653,7 @@
   <dimension ref="A1:L23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:K6"/>
+      <selection activeCell="A8" sqref="A8:K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -667,14 +667,14 @@
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
-      <c r="E1" s="14" t="s">
+      <c r="E1" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="F1" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14" t="s">
+      <c r="G1" s="18"/>
+      <c r="H1" s="18" t="s">
         <v>4</v>
       </c>
       <c r="I1" s="2"/>
@@ -687,10 +687,10 @@
       <c r="B2" s="3"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
@@ -704,13 +704,13 @@
       <c r="E3" s="4">
         <v>678</v>
       </c>
-      <c r="F3" s="16">
+      <c r="F3" s="20">
         <f>(H3/E3)</f>
-        <v>3.1415929203539825</v>
-      </c>
-      <c r="G3" s="17"/>
+        <v>1.0516224188790559</v>
+      </c>
+      <c r="G3" s="21"/>
       <c r="H3" s="5">
-        <v>2130</v>
+        <v>713</v>
       </c>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
@@ -722,95 +722,95 @@
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
-      <c r="E4" s="11" t="s">
+      <c r="E4" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11" t="s">
+      <c r="F4" s="15"/>
+      <c r="G4" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="H4" s="11"/>
+      <c r="H4" s="15"/>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
     </row>
     <row r="5" spans="1:12" ht="27.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A5" s="20" t="s">
+      <c r="A5" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="20"/>
+      <c r="B5" s="12"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
-      <c r="E5" s="12">
+      <c r="E5" s="16">
         <v>136</v>
       </c>
-      <c r="F5" s="13"/>
-      <c r="G5" s="8">
+      <c r="F5" s="17"/>
+      <c r="G5" s="10">
         <f>(E5*F3)</f>
-        <v>427.25663716814165</v>
-      </c>
-      <c r="H5" s="9"/>
+        <v>143.02064896755161</v>
+      </c>
+      <c r="H5" s="11"/>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
       <c r="L5" s="2"/>
     </row>
     <row r="6" spans="1:12" ht="8.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="10"/>
-      <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="10"/>
-      <c r="J6" s="10"/>
-      <c r="K6" s="10"/>
+      <c r="A6" s="14"/>
+      <c r="B6" s="14"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="14"/>
+      <c r="K6" s="14"/>
       <c r="L6" s="2"/>
     </row>
     <row r="7" spans="1:12" ht="27.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A7" s="20" t="s">
+      <c r="A7" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="21"/>
-      <c r="C7" s="18">
-        <v>0.3</v>
-      </c>
-      <c r="D7" s="19"/>
-      <c r="E7" s="8">
+      <c r="B7" s="13"/>
+      <c r="C7" s="8">
+        <v>0.4</v>
+      </c>
+      <c r="D7" s="9"/>
+      <c r="E7" s="10">
         <f>(E3*C7)</f>
-        <v>203.4</v>
-      </c>
-      <c r="F7" s="9"/>
-      <c r="G7" s="8">
+        <v>271.2</v>
+      </c>
+      <c r="F7" s="11"/>
+      <c r="G7" s="10">
         <f>((E3*C7)*F3)</f>
-        <v>639.00000000000011</v>
-      </c>
-      <c r="H7" s="9"/>
+        <v>285.19999999999993</v>
+      </c>
+      <c r="H7" s="11"/>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
     </row>
     <row r="8" spans="1:12" ht="8.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="10"/>
-      <c r="B8" s="10"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="10"/>
-      <c r="I8" s="10"/>
-      <c r="J8" s="10"/>
-      <c r="K8" s="10"/>
+      <c r="A8" s="14"/>
+      <c r="B8" s="14"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="14"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="14"/>
+      <c r="K8" s="14"/>
       <c r="L8" s="2"/>
     </row>
     <row r="9" spans="1:12" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A9" s="20"/>
-      <c r="B9" s="20"/>
+      <c r="A9" s="12"/>
+      <c r="B9" s="12"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
@@ -1016,12 +1016,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A8:K8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="G7:H7"/>
     <mergeCell ref="G5:H5"/>
     <mergeCell ref="A6:K6"/>
     <mergeCell ref="E4:F4"/>
@@ -1032,6 +1026,12 @@
     <mergeCell ref="F3:G3"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="G4:H4"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:K8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="G7:H7"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>